<commit_message>
Cooley-Tukey Radix 2 FFT - Fix test case
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/CooleyTukeyRadix2Test.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/CooleyTukeyRadix2Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pure Real 10" sheetId="1" r:id="rId1"/>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,32 +1679,32 @@
         <v>80.989178161394591</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" ref="J19:P19" si="13">J9-J13</f>
-        <v>-64.093137274202746</v>
+        <f t="shared" ref="J19:P19" si="13">B9-J13</f>
+        <v>-212.06084894742182</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="13"/>
-        <v>-116.10516989677649</v>
+        <v>-132.09314861453308</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" si="13"/>
-        <v>-7.5079105150806811</v>
+        <v>-117.13597459701981</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="13"/>
-        <v>-37.106244620886741</v>
+        <v>141.74787818135908</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="13"/>
-        <v>230.91517080259121</v>
+        <v>85.158694752799903</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="13"/>
-        <v>303.36568058488206</v>
+        <v>253.93505672202761</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="13"/>
-        <v>365.72111208270621</v>
+        <v>379.46237715627058</v>
       </c>
       <c r="Q19" t="s">
         <v>8</v>
@@ -2408,7 +2408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="M20" sqref="M20:X20"/>
     </sheetView>
   </sheetViews>
@@ -3107,7 +3107,7 @@
         <v>-135.55074381473719</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" ref="M20:T20" si="16">A10-M15</f>
+        <f t="shared" ref="M20" si="16">A10-M15</f>
         <v>49.079987433711921</v>
       </c>
       <c r="N20" s="2">
@@ -3176,1381 +3176,1381 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*256-128</f>
-        <v>-67.656533509529311</v>
+        <v>-82.658595982563298</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:K16" ca="1" si="0">RAND()*256-128</f>
-        <v>-64.512690149394473</v>
+        <v>-24.636956967373749</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7859820661110177</v>
+        <v>80.643481916166309</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-125.10388700937131</v>
+        <v>104.27903193772337</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-59.630281436231769</v>
+        <v>-47.049411604327588</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>14.136816851837921</v>
+        <v>38.170398578129465</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>64.100474830793104</v>
+        <v>88.302317665672433</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>-124.53551904917848</v>
+        <v>87.740497796241812</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>117.7821528619875</v>
+        <v>-70.335452002680768</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>73.9985812694743</v>
+        <v>60.778677125830853</v>
       </c>
       <c r="K1">
         <f t="shared" ca="1" si="0"/>
-        <v>-23.619635035259535</v>
+        <v>13.768702635112646</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:K30" ca="1" si="1">RAND()*256-128</f>
-        <v>56.761437048160133</v>
+        <v>99.299565445463401</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>10.526615851966</v>
+        <v>41.126921154925327</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>104.67286816982485</v>
+        <v>-99.344899276068048</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>-42.856979226599066</v>
+        <v>75.755422227322811</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-73.044645265388084</v>
+        <v>92.456213627177419</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>98.032930538341361</v>
+        <v>20.960396142849618</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>70.874462767696059</v>
+        <v>126.11479228838721</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>40.568437005345316</v>
+        <v>20.286083292816727</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>114.47324806320441</v>
+        <v>73.430262875033009</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2579351604515239</v>
+        <v>99.316587895321902</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>35.27661353537917</v>
+        <v>108.68955955719036</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-117.69619397380814</v>
+        <v>-80.629090954974401</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>26.435052654851319</v>
+        <v>42.164610035298125</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-62.751383306067197</v>
+        <v>-48.873247089802874</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.9245995735803945</v>
+        <v>-100.23911498692627</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-37.21365738255318</v>
+        <v>113.97682140974931</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-30.201630256945464</v>
+        <v>-0.33908669666959668</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>-99.874595778065242</v>
+        <v>92.648310626251856</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25108403643210409</v>
+        <v>19.821512196331383</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-103.3569308352811</v>
+        <v>45.405295774244479</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>39.646214863870256</v>
+        <v>-115.19748523147553</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>100.383792369513</v>
+        <v>-123.35244189452354</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>-45.765373337596259</v>
+        <v>40.09332403570798</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-33.951733008436435</v>
+        <v>-104.80943627960832</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-112.04041702856924</v>
+        <v>-115.40991224907489</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-116.55943798876166</v>
+        <v>-111.21493096816596</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>-46.768204696965938</v>
+        <v>116.20731647545756</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-66.964213173080992</v>
+        <v>37.774598884317783</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-74.549120169540004</v>
+        <v>-5.635676816221121</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>94.364081780221824</v>
+        <v>12.661842824942084</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>84.367668736839335</v>
+        <v>94.462474770748457</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>-92.253285842289444</v>
+        <v>86.914445819072427</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>49.317172689755012</v>
+        <v>12.439669498578496</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>125.44289109519238</v>
+        <v>55.800059565293509</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>50.268509036828277</v>
+        <v>91.29828038830118</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.613688082775667</v>
+        <v>-8.4190391544895533</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>67.908621133141594</v>
+        <v>-15.99028353779596</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>88.96319760190363</v>
+        <v>46.074024083404254</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>33.138263272567997</v>
+        <v>-73.72753594742764</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>45.195429522700522</v>
+        <v>17.501769865184599</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.4514147314612558</v>
+        <v>-127.14948290999396</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.929994137728158</v>
+        <v>-78.281534029778385</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>120.42054801841331</v>
+        <v>-45.624413205677541</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>7.837225885239036</v>
+        <v>-21.572554312181921</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-84.99179572550517</v>
+        <v>-71.556898227851661</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-75.629543406404622</v>
+        <v>-113.79912837122217</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-75.365498776392542</v>
+        <v>64.680320335775548</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3981313844088845</v>
+        <v>14.857856567566898</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>54.978805943925806</v>
+        <v>57.146690573986945</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-85.014008189150843</v>
+        <v>-114.62709843051084</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>21.625671954050347</v>
+        <v>118.81930468530209</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>123.2453684842524</v>
+        <v>-118.48211945477428</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>23.714646396953242</v>
+        <v>-104.49353247525914</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>14.544321299904368</v>
+        <v>-90.896342718642728</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>-103.43389196213082</v>
+        <v>93.063994444881189</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5413747240549185</v>
+        <v>90.258078900792583</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-76.011206296761344</v>
+        <v>-94.140880152318175</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-53.734947919130093</v>
+        <v>70.499893264874061</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>-108.70056738110475</v>
+        <v>5.0797348047202036</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>-61.89108380751378</v>
+        <v>45.31347685096469</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-77.675144492406758</v>
+        <v>39.89438565874562</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>13.120584307992004</v>
+        <v>-61.353663004161831</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>59.970792468149853</v>
+        <v>-11.635004609928075</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>-36.48879721900596</v>
+        <v>-80.219815685354831</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>44.868553061744961</v>
+        <v>-76.96273372861873</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9801970547236465</v>
+        <v>97.39732296496075</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>40.160783055675864</v>
+        <v>19.605833216716064</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>33.876086437483366</v>
+        <v>-28.612493700827173</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-80.291915773462648</v>
+        <v>70.96220745665039</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>112.26054964346812</v>
+        <v>124.70932036769301</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-73.22932813129583</v>
+        <v>103.52865208816354</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>-40.0005115870662</v>
+        <v>105.68302611529145</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-48.434836795621436</v>
+        <v>-127.67970590964273</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>-109.00906801847881</v>
+        <v>41.240388881348679</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.835059967302925</v>
+        <v>-77.383887465291679</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.512362887223361</v>
+        <v>-39.123230908581064</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>-120.84779839600651</v>
+        <v>67.949664168363967</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>16.719908758385969</v>
+        <v>-109.70286539211398</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-100.25782327484754</v>
+        <v>-112.50180214340054</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-97.74714670789362</v>
+        <v>78.499339266253003</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>50.668769190111846</v>
+        <v>-18.104614675162168</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-26.432677825878272</v>
+        <v>57.29371158304653</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>41.326195459638626</v>
+        <v>-62.627972921859254</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>117.44995261348913</v>
+        <v>-51.863011706722006</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>27.919576361452869</v>
+        <v>30.672271658008384</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>-112.35032447458866</v>
+        <v>-36.45978180202232</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>-103.87717457072935</v>
+        <v>84.989134708905794</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>-76.674076241857534</v>
+        <v>19.892125335799733</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>121.67291597841484</v>
+        <v>-89.064502465711058</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>82.049829601944197</v>
+        <v>-55.042816498166559</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>65.563207908370714</v>
+        <v>58.281715675106852</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-108.64402976646369</v>
+        <v>-79.877194111457243</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-114.20998911477673</v>
+        <v>20.147581696862431</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-63.461518072119674</v>
+        <v>118.66081801884241</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.249307512487405</v>
+        <v>29.505148501685255</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>101.30049810847609</v>
+        <v>71.553073687689249</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>33.097222919787953</v>
+        <v>35.771443886865342</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.760125757473674</v>
+        <v>-38.656452098195871</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>-114.94007497829188</v>
+        <v>-27.455997284604422</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-22.962842939653399</v>
+        <v>-95.297401033456566</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>86.929439840552675</v>
+        <v>46.280815158059738</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>20.743695069657576</v>
+        <v>87.233456189996332</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.315918171792305</v>
+        <v>97.282693595791358</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>87.41515868304549</v>
+        <v>119.12564257117961</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>39.604681620477578</v>
+        <v>84.736741485826741</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>-43.734131807949467</v>
+        <v>63.300332743768081</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-126.54464010205967</v>
+        <v>19.485034179558056</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>16.721606248693945</v>
+        <v>4.4961917463492114</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>-26.457744736606145</v>
+        <v>30.563065032243401</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>82.590000307305303</v>
+        <v>-93.284523648112923</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>11.135173440627142</v>
+        <v>35.044665158944525</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>62.724035527479117</v>
+        <v>22.534517891685852</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>45.730384840402593</v>
+        <v>43.888509445342976</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.149519115756078</v>
+        <v>66.756105610260192</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>117.82387880027699</v>
+        <v>34.597723955637207</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>34.918361081348991</v>
+        <v>-85.172299909076486</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>26.765536874738444</v>
+        <v>43.287760802482438</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>105.74145406982194</v>
+        <v>-54.6100940132647</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>-125.22808981452658</v>
+        <v>119.21947166876109</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>37.145913567945058</v>
+        <v>126.98917637311135</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>-73.390863217256367</v>
+        <v>90.047227501907344</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.742070638756928</v>
+        <v>-76.56912523172241</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-111.08230300910375</v>
+        <v>44.929597990724517</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>105.18071514656191</v>
+        <v>-27.822023549827946</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.2461157103105904</v>
+        <v>-49.458442488693208</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>122.95009060298653</v>
+        <v>116.75016200231909</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>20.181732102720929</v>
+        <v>-63.964052076420842</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>25.578412470666308</v>
+        <v>-8.6569054419026656</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>69.687584720786646</v>
+        <v>-124.41711582577261</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>26.698280938293976</v>
+        <v>82.312153442606302</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>90.8338205050309</v>
+        <v>-65.264104858096431</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>125.12614204102226</v>
+        <v>98.99790038692521</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-105.2361284431403</v>
+        <v>41.288054519790222</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>10.381244942131758</v>
+        <v>-42.806317795263283</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-39.649591046170428</v>
+        <v>101.76863525276522</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>-124.18706688258382</v>
+        <v>54.570142156707249</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-118.52604812319817</v>
+        <v>27.947742643240701</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>55.839778118904235</v>
+        <v>127.79267491720705</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-108.91648702247602</v>
+        <v>-15.890333980755855</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3148830275094099</v>
+        <v>127.65371068711477</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-42.567703894424</v>
+        <v>-85.009290872686449</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.2408208185021294</v>
+        <v>-116.81806939870927</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>-109.65607181032419</v>
+        <v>4.727272255969325</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-58.844044864625431</v>
+        <v>61.44736048942562</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>105.47797655551304</v>
+        <v>-78.974153469641664</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-75.898842960562547</v>
+        <v>-121.97716323140546</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>-28.036314347456852</v>
+        <v>-84.775946216434534</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-63.096042726030561</v>
+        <v>29.197965249570842</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-80.151991808209146</v>
+        <v>-120.34345566048901</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>14.001769815493759</v>
+        <v>56.613020726739194</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>32.448267419941686</v>
+        <v>18.805997654321288</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-124.52062841939943</v>
+        <v>-107.8636530165291</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>43.154652325403049</v>
+        <v>117.08445921947998</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>28.042341667725282</v>
+        <v>57.745917357106862</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>-54.510998611841728</v>
+        <v>18.112268217666923</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>80.164044830938508</v>
+        <v>-49.797168369911759</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>101.40171167697736</v>
+        <v>-35.766883645395808</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>44.826242817249977</v>
+        <v>36.795514398132468</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>57.499116769768108</v>
+        <v>-33.607118028072904</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>12.16784054984825</v>
+        <v>-107.14035786460036</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>68.290121424566109</v>
+        <v>61.120429996709419</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>-105.31963246519481</v>
+        <v>76.234864559599089</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>35.975027192847534</v>
+        <v>-118.3069000038349</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>104.40084169240708</v>
+        <v>-49.971918500764133</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>107.50607311896329</v>
+        <v>-40.187149092563828</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>-67.808804135789842</v>
+        <v>37.667872698970598</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>-36.942538698799439</v>
+        <v>55.837216604472133</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>-127.43370278845256</v>
+        <v>-126.60240882274201</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>47.298854688832762</v>
+        <v>-67.084558998970778</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-41.18445546149448</v>
+        <v>-107.07689572897451</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-57.543099370362768</v>
+        <v>108.10209836728777</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.58089614420106273</v>
+        <v>-109.8849219489594</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>-80.787689831703148</v>
+        <v>52.343891679180359</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>64.526066419197406</v>
+        <v>121.34786394521333</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>-77.784056699181377</v>
+        <v>23.137916604270913</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>90.681161273835897</v>
+        <v>-86.725494012375378</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.1650521649393681</v>
+        <v>13.232731065578946</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-87.192532958555233</v>
+        <v>-124.0078995050807</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>21.844915894549104</v>
+        <v>-127.84360073209874</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-98.678329119796189</v>
+        <v>41.75296928457638</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.06468880930322</v>
+        <v>0.2189041566811909</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>33.101056569591066</v>
+        <v>-109.40993310098906</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-83.545006231931893</v>
+        <v>-76.118511304586292</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8936121194675195</v>
+        <v>121.44734689847053</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.477942611689002</v>
+        <v>-119.70110731753144</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>78.088319235724072</v>
+        <v>16.578942475554982</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>99.78230249589032</v>
+        <v>77.096705355596725</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>-118.38017982733524</v>
+        <v>-101.97896584864171</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-98.121839509753926</v>
+        <v>-5.6411022001688877</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>89.563723843901528</v>
+        <v>119.33328927987554</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>40.337599395680314</v>
+        <v>-62.418807642947002</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.700624944361579</v>
+        <v>54.290220469603582</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>60.65382632340183</v>
+        <v>-114.93555509968127</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>58.566073854105809</v>
+        <v>-118.61529084484985</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>-31.130549100802568</v>
+        <v>114.25656809148958</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>-126.80893286856653</v>
+        <v>-31.341974579445917</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>93.541502186376647</v>
+        <v>-43.575416045630561</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>-52.050850298890197</v>
+        <v>-22.908008255068182</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>122.71071354063852</v>
+        <v>75.190135392809026</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>78.639852206485898</v>
+        <v>-124.76497762231716</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-92.422514834378291</v>
+        <v>-45.401007836400879</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>-116.56898298605498</v>
+        <v>94.172443190938964</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-114.94150956505757</v>
+        <v>-48.695358927830455</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-64.089573467505375</v>
+        <v>-35.82522792318079</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>66.405516786093841</v>
+        <v>17.657940947519762</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>-88.893608842046575</v>
+        <v>70.367214008081561</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>-49.740410040121787</v>
+        <v>-28.407170871902281</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>71.271253494375088</v>
+        <v>85.546746296230566</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>126.9965922316978</v>
+        <v>57.438072471257129</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>126.41487727132449</v>
+        <v>58.296588826786916</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0314177931481368</v>
+        <v>60.564356483681195</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>90.134374262334603</v>
+        <v>-6.4417722993547102</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>-94.695410167272598</v>
+        <v>-89.043875846039725</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>-43.101219876700071</v>
+        <v>12.071351636258072</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7065967647118612</v>
+        <v>-26.710006856537149</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>-39.483890157650478</v>
+        <v>-42.355083860108152</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>73.091828896911096</v>
+        <v>29.995675669991385</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>106.00991673933487</v>
+        <v>127.24221756680979</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>-120.55330358401233</v>
+        <v>15.285358900089335</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>81.899273404774448</v>
+        <v>92.331673686108644</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>45.097536181102868</v>
+        <v>106.98984437073824</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>103.2330178363359</v>
+        <v>-75.650482903079961</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>-25.202718118158344</v>
+        <v>64.900922227830165</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>-60.140626128679912</v>
+        <v>41.050831174982108</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.505028956835474</v>
+        <v>33.818410035313889</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>80.170107998128913</v>
+        <v>62.88697576530069</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>44.856624892739973</v>
+        <v>-93.27904574994119</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>-59.42519256983374</v>
+        <v>-116.57285009333137</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>116.01335274890081</v>
+        <v>103.81780136042633</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>115.48165551003825</v>
+        <v>71.094072516360484</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>-112.99646422572735</v>
+        <v>18.973813550488245</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>-75.085719947096237</v>
+        <v>116.2658361122414</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.569084985866084</v>
+        <v>61.394875858001512</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4722226912703604</v>
+        <v>59.363370356378454</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>123.7769898807496</v>
+        <v>61.583677522731506</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>-43.04167815699779</v>
+        <v>72.44398738718138</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>22.628486354940776</v>
+        <v>51.552361537576672</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>-48.199340934779826</v>
+        <v>100.46574361603786</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>96.519522694029519</v>
+        <v>85.106208371018965</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>69.323718177253141</v>
+        <v>-38.518745247937744</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>-34.390300557388485</v>
+        <v>-76.742245473051213</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>63.227907895503591</v>
+        <v>5.848257294608203</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>-90.50488965496325</v>
+        <v>38.129240198545091</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>21.833157829691999</v>
+        <v>-119.87451248751847</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>87.547767082657401</v>
+        <v>-105.44469842525746</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>64.70955679669413</v>
+        <v>-12.134549323232648</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>-76.729869814097128</v>
+        <v>-75.415651799687026</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>54.734436053190194</v>
+        <v>56.751368301077321</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.022985314624492</v>
+        <v>-91.249556269196944</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.9360701570522</v>
+        <v>-7.0642636553282045</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>-80.21829167914089</v>
+        <v>22.627167989317456</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>117.06897104038563</v>
+        <v>84.163828711075411</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>-50.506252662067595</v>
+        <v>72.56790020729278</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-78.485343872587634</v>
+        <v>-16.605521500185063</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.220083352351679</v>
+        <v>-115.74626336913326</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.8591908959431862</v>
+        <v>-72.142984031451022</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.8688807125702738</v>
+        <v>38.380855957539666</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>72.389342873623576</v>
+        <v>43.623524095832238</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-30.436932486487478</v>
+        <v>-88.935594957450462</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>-52.051034517593649</v>
+        <v>99.293132714088983</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>61.850196695952661</v>
+        <v>-60.69759858673504</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>27.979470422607989</v>
+        <v>-110.63790271007994</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>88.99424600987183</v>
+        <v>55.330425978526819</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>-71.464792784518011</v>
+        <v>66.594554247123597</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>-71.323002460950192</v>
+        <v>83.877835106712467</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>-108.02049099624145</v>
+        <v>59.508055869629345</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>55.165982063498632</v>
+        <v>-77.942748622278771</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>-20.011463480597996</v>
+        <v>62.815491139049499</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>-35.784007882638889</v>
+        <v>30.405101557493225</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>62.612321845569141</v>
+        <v>25.516960777510661</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>-80.587749215476975</v>
+        <v>78.443928416995533</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>39.24636387356307</v>
+        <v>25.497924906483689</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>-76.716194769531938</v>
+        <v>-107.34744919448801</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>49.429985376438225</v>
+        <v>72.111923464870728</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="1"/>
-        <v>-92.902003214940123</v>
+        <v>-13.074929193786119</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>-68.854654764315171</v>
+        <v>63.1632926963008</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>-113.90100845474527</v>
+        <v>9.8206069898160138</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>-52.546446598813361</v>
+        <v>92.154789331342641</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>-80.406183605083072</v>
+        <v>2.0839163280500657</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>-35.399519543661711</v>
+        <v>53.948299892419385</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>110.92473213129804</v>
+        <v>62.31203959473703</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>-46.699305697170274</v>
+        <v>112.9132190043031</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31428679942536064</v>
+        <v>-81.389288247764341</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.207187036545918</v>
+        <v>-114.1463665840391</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>-56.272284811185699</v>
+        <v>81.563620491451644</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="1"/>
-        <v>69.388214038932205</v>
+        <v>-35.311760626025972</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>-78.73958413919928</v>
+        <v>26.860132990254272</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>-84.800857354846244</v>
+        <v>8.3909607513137132</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>-92.57277511752568</v>
+        <v>44.332817314682643</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>-92.824453485906588</v>
+        <v>33.929303237832983</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>33.103773872036612</v>
+        <v>-23.03804030988988</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>-111.1609603568092</v>
+        <v>43.441504941425706</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>-47.312464903283342</v>
+        <v>57.134668847613909</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>90.964477313776513</v>
+        <v>-100.43085215554473</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>64.359914183271428</v>
+        <v>-24.827495028169238</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>126.97123111108763</v>
+        <v>51.074376421334961</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="1"/>
-        <v>-65.13323023745923</v>
+        <v>-90.315642815846729</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>18.51546429840144</v>
+        <v>-35.303072144800012</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>48.404419032749701</v>
+        <v>-28.729751011199795</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>83.282501802659453</v>
+        <v>0.66672704048301057</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>-48.66795559789864</v>
+        <v>-4.6969698361345422</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3733893265100789</v>
+        <v>41.614396329410056</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>74.892141381116488</v>
+        <v>-100.71892371841415</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>110.37607764076944</v>
+        <v>53.856999461419065</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>-36.819732276405944</v>
+        <v>76.218507451292936</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>-102.00936202292323</v>
+        <v>-4.4376527943476844</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="1"/>
-        <v>-120.10884569056529</v>
+        <v>42.441883323436798</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="1"/>
-        <v>-93.89366870835417</v>
+        <v>4.8664362031431665</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>14.877537235710491</v>
+        <v>60.502237893490673</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>-81.289794510805024</v>
+        <v>-10.631946920304614</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>117.49656557098928</v>
+        <v>-78.450357641969163</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>-31.558022593084161</v>
+        <v>30.913689582913008</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31541378717770385</v>
+        <v>97.998286403582199</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>-68.031050638809972</v>
+        <v>-82.434833721002917</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>-91.003386791799898</v>
+        <v>45.169645689738815</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>-90.319884765681678</v>
+        <v>-58.310366402398699</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>3.570330177207893</v>
+        <v>-35.401035326062271</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="1"/>
-        <v>-53.351464027825244</v>
+        <v>-66.703768346529529</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="1"/>
-        <v>56.617055584978687</v>
+        <v>25.337527484306662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cooley Tukey FFT and Tests
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/CooleyTukeyRadix2Test.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/CooleyTukeyRadix2Test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\jacobi\jacobi\src\test\resources\jacobi\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Pure Real 10" sheetId="1" r:id="rId1"/>
@@ -13,14 +18,15 @@
     <sheet name="Complex 6" sheetId="6" r:id="rId4"/>
     <sheet name="Complex 8" sheetId="7" r:id="rId5"/>
     <sheet name="Complex 24" sheetId="8" r:id="rId6"/>
-    <sheet name="rand" sheetId="3" r:id="rId7"/>
+    <sheet name="Complex 10 DFT" sheetId="9" r:id="rId7"/>
+    <sheet name="rand" sheetId="3" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
   <si>
     <t>Cos</t>
   </si>
@@ -62,6 +68,42 @@
   </si>
   <si>
     <t>Imag</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>Im</t>
+  </si>
+  <si>
+    <t>DFT-10 Matrix</t>
+  </si>
+  <si>
+    <t>Re(F)*Re(v)</t>
+  </si>
+  <si>
+    <t>Re(F)*Im(v)</t>
+  </si>
+  <si>
+    <t>Im(F)*Re(v)</t>
+  </si>
+  <si>
+    <t>Im(F)*Im(v)</t>
+  </si>
+  <si>
+    <t>DFT-10</t>
+  </si>
+  <si>
+    <t>Group 2-by-2</t>
+  </si>
+  <si>
+    <t>DFT-5 Matrix</t>
+  </si>
+  <si>
+    <t>DFT-5 of 2 Groups</t>
   </si>
 </sst>
 </file>
@@ -124,6 +166,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -171,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,7 +251,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1249,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I20" sqref="I20:P20"/>
     </sheetView>
   </sheetViews>
@@ -3165,10 +3210,1981 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>66.826034951722022</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-77.321397401765495</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-13.723181668720144</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-83.274074566265881</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-80.138195486362974</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-44.485991069977388</v>
+      </c>
+      <c r="G2" s="1">
+        <v>34.707742945432244</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-100.28633196555467</v>
+      </c>
+      <c r="I2" s="1">
+        <v>50.286550686922311</v>
+      </c>
+      <c r="J2" s="2">
+        <v>104.63349386330464</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>-79.984863734409032</v>
+      </c>
+      <c r="B3" s="2">
+        <v>38.484590266675468</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-124.99230072723466</v>
+      </c>
+      <c r="D3" s="2">
+        <v>86.840397082432276</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-16.99864451313141</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-53.559455663745553</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-107.98901568065543</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-107.16794995062781</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-76.126079331176356</v>
+      </c>
+      <c r="J3" s="2">
+        <v>29.469237660107098</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>7</v>
+      </c>
+      <c r="V7">
+        <v>8</v>
+      </c>
+      <c r="W7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <f>COS(B$7*$A8*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:K17" si="0">COS(C$7*$A8*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>COS(J$7*$A8*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>-SIN(N$7*$A8*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:W17" si="1">-SIN(O$7*$A8*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B17" si="2">COS(B$7*$A9*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494745</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494745</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494734</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494734</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494756</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494734</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:N17" si="3">-SIN(N$7*$A9*2*PI()/COUNTA($B$7:$K$7))</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247314</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515364</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247325</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>-1.22514845490862E-16</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247303</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515353</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494745</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494734</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494773</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494723</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494767</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494701</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247325</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247303</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="1"/>
+        <v>2.45029690981724E-16</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247336</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="1"/>
+        <v>0.5877852522924728</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494734</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494734</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494773</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494701</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494767</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494712</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494806</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515364</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247303</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247336</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>-3.67544536472586E-16</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515375</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247269</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247358</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494734</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494773</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494767</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494712</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494679</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494817</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-0.8090169943749479</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247325</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>0.5877852522924728</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>4.90059381963448E-16</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247358</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515375</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515331</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>-1.22514845490862E-16</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>2.45029690981724E-16</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>-3.67544536472586E-16</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>4.90059381963448E-16</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>-6.1257422745431001E-16</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>7.3508907294517201E-16</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="1"/>
+        <v>-8.5760391843603401E-16</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>9.8011876392689601E-16</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="1"/>
+        <v>-1.102633609417758E-15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494773</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494701</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494712</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>-0.8090169943749479</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494839</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494629</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494667</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247303</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515375</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247358</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>7.3508907294517201E-16</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247247</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515331</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515398</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247425</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494756</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494723</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494767</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494679</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494839</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494468</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494823</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494934</v>
+      </c>
+      <c r="M15">
+        <v>7</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515353</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247336</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247269</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515375</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>-8.5760391843603401E-16</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515331</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247702</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247203</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494767</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494712</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494817</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494629</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494823</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494645</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494912</v>
+      </c>
+      <c r="M16">
+        <v>8</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>0.5877852522924728</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247358</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515331</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>9.8011876392689601E-16</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515398</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247203</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247436</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.80901699437494734</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494701</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494806</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>-0.8090169943749479</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>-0.80901699437494667</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>-0.30901699437494934</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0.30901699437494912</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>0.80901699437495067</v>
+      </c>
+      <c r="M17">
+        <v>9</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247336</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515375</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="1"/>
+        <v>0.95105651629515342</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>0.58778525229247247</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>-1.102633609417758E-15</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>-0.58778525229247425</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515298</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="1"/>
+        <v>-0.95105651629515298</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="1"/>
+        <v>-0.5877852522924687</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="array" ref="A19:J19">TRANSPOSE(MMULT(B8:K17,TRANSPOSE(A2:J2)))</f>
+        <v>-142.77534971126536</v>
+      </c>
+      <c r="B19">
+        <v>238.18397188978344</v>
+      </c>
+      <c r="C19">
+        <v>135.66426541436488</v>
+      </c>
+      <c r="D19">
+        <v>-89.250533120161208</v>
+      </c>
+      <c r="E19">
+        <v>-8.4264808543706096</v>
+      </c>
+      <c r="F19">
+        <v>258.69325256925225</v>
+      </c>
+      <c r="G19">
+        <v>-8.4264808543707375</v>
+      </c>
+      <c r="H19">
+        <v>-89.250533120160981</v>
+      </c>
+      <c r="I19">
+        <v>135.6642654143651</v>
+      </c>
+      <c r="J19">
+        <v>238.18397188978423</v>
+      </c>
+      <c r="K19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="array" ref="A20:J20">TRANSPOSE(MMULT(B8:K17,TRANSPOSE(A3:J3)))</f>
+        <v>-412.02408459176536</v>
+      </c>
+      <c r="B20">
+        <v>73.800096709988352</v>
+      </c>
+      <c r="C20">
+        <v>27.984780249850246</v>
+      </c>
+      <c r="D20">
+        <v>60.215244804077166</v>
+      </c>
+      <c r="E20">
+        <v>-155.83353644935403</v>
+      </c>
+      <c r="F20">
+        <v>-400.15772338144836</v>
+      </c>
+      <c r="G20">
+        <v>-155.83353644935409</v>
+      </c>
+      <c r="H20">
+        <v>60.215244804077386</v>
+      </c>
+      <c r="I20">
+        <v>27.984780249850516</v>
+      </c>
+      <c r="J20">
+        <v>73.800096709988367</v>
+      </c>
+      <c r="K20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="array" ref="A21:J21">TRANSPOSE(MMULT(N8:W17,TRANSPOSE(A2:J2)))</f>
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>219.15240537064585</v>
+      </c>
+      <c r="C21">
+        <v>111.44793758317067</v>
+      </c>
+      <c r="D21">
+        <v>254.64994045068232</v>
+      </c>
+      <c r="E21">
+        <v>-37.61083854743643</v>
+      </c>
+      <c r="F21">
+        <v>7.0129479031342516E-14</v>
+      </c>
+      <c r="G21">
+        <v>37.610838547436217</v>
+      </c>
+      <c r="H21">
+        <v>-254.64994045068275</v>
+      </c>
+      <c r="I21">
+        <v>-111.44793758317054</v>
+      </c>
+      <c r="J21">
+        <v>-219.15240537064534</v>
+      </c>
+      <c r="K21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="array" ref="A22:J22">TRANSPOSE(MMULT(N8:W17,TRANSPOSE(A3:J3)))</f>
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>-196.82025395524664</v>
+      </c>
+      <c r="C22">
+        <v>220.72096505534799</v>
+      </c>
+      <c r="D22">
+        <v>-9.7986943263527984</v>
+      </c>
+      <c r="E22">
+        <v>-182.80373398035474</v>
+      </c>
+      <c r="F22">
+        <v>-1.373609372747435E-13</v>
+      </c>
+      <c r="G22">
+        <v>182.80373398035471</v>
+      </c>
+      <c r="H22">
+        <v>9.7986943263525426</v>
+      </c>
+      <c r="I22">
+        <v>-220.72096505534776</v>
+      </c>
+      <c r="J22">
+        <v>196.82025395524684</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>A19-A22</f>
+        <v>-142.77534971126536</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ref="B27:J27" si="4">B19-B22</f>
+        <v>435.00422584503008</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="4"/>
+        <v>-85.056699640983112</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>-79.451838793808406</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>174.37725312598411</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>258.69325256925237</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>-191.23021483472544</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>-99.049227446513527</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>356.38523046971284</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="4"/>
+        <v>41.363717934537391</v>
+      </c>
+      <c r="K27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>A20+A21</f>
+        <v>-412.02408459176536</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ref="B28:J28" si="5">B20+B21</f>
+        <v>292.95250208063419</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="5"/>
+        <v>139.43271783302092</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="5"/>
+        <v>314.86518525475947</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="5"/>
+        <v>-193.44437499679046</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>-400.15772338144831</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>-118.22269790191787</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="5"/>
+        <v>-194.43469564660535</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>-83.463157333320027</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>-145.35230866065697</v>
+      </c>
+      <c r="K28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f>A2</f>
+        <v>66.826034951722022</v>
+      </c>
+      <c r="B32" s="1">
+        <f>C2</f>
+        <v>-13.723181668720144</v>
+      </c>
+      <c r="C32" s="1">
+        <f>E2</f>
+        <v>-80.138195486362974</v>
+      </c>
+      <c r="D32" s="1">
+        <f>G2</f>
+        <v>34.707742945432244</v>
+      </c>
+      <c r="E32" s="1">
+        <f>I2</f>
+        <v>50.286550686922311</v>
+      </c>
+      <c r="F32" s="2">
+        <f>B2</f>
+        <v>-77.321397401765495</v>
+      </c>
+      <c r="G32" s="2">
+        <f>D2</f>
+        <v>-83.274074566265881</v>
+      </c>
+      <c r="H32" s="2">
+        <f>F2</f>
+        <v>-44.485991069977388</v>
+      </c>
+      <c r="I32" s="2">
+        <f>H2</f>
+        <v>-100.28633196555467</v>
+      </c>
+      <c r="J32" s="2">
+        <f>J2</f>
+        <v>104.63349386330464</v>
+      </c>
+      <c r="K32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f>A3</f>
+        <v>-79.984863734409032</v>
+      </c>
+      <c r="B33" s="1">
+        <f>C3</f>
+        <v>-124.99230072723466</v>
+      </c>
+      <c r="C33" s="1">
+        <f>E3</f>
+        <v>-16.99864451313141</v>
+      </c>
+      <c r="D33" s="1">
+        <f>G3</f>
+        <v>-107.98901568065543</v>
+      </c>
+      <c r="E33" s="1">
+        <f>I3</f>
+        <v>-76.126079331176356</v>
+      </c>
+      <c r="F33" s="2">
+        <f>B3</f>
+        <v>38.484590266675468</v>
+      </c>
+      <c r="G33" s="2">
+        <f>D3</f>
+        <v>86.840397082432276</v>
+      </c>
+      <c r="H33" s="2">
+        <f>F3</f>
+        <v>-53.559455663745553</v>
+      </c>
+      <c r="I33" s="2">
+        <f>H3</f>
+        <v>-107.16794995062781</v>
+      </c>
+      <c r="J33" s="2">
+        <f>J3</f>
+        <v>29.469237660107098</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>3</v>
+      </c>
+      <c r="M36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ref="B37:F41" si="6">COS(B$7*$A37*2*PI()/COUNTA($B$36:$F$36))</f>
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f>-SIN(I$36*$A37*2*PI()/COUNTA($I$36:$M$36))</f>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:M41" si="7">-SIN(J$36*$A37*2*PI()/COUNTA($I$36:$M$36))</f>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494745</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494734</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38:I41" si="8">-SIN(I$36*$A38*2*PI()/COUNTA($I$36:$M$36))</f>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="7"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="7"/>
+        <v>-0.58778525229247325</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="7"/>
+        <v>0.58778525229247303</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="7"/>
+        <v>0.95105651629515364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494734</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494773</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494767</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="7"/>
+        <v>-0.58778525229247325</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="7"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="7"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="7"/>
+        <v>0.5877852522924728</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494756</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494773</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494701</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494712</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="7"/>
+        <v>0.58778525229247303</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="7"/>
+        <v>-0.95105651629515353</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="7"/>
+        <v>0.95105651629515375</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="7"/>
+        <v>-0.58778525229247358</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494723</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494767</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="6"/>
+        <v>-0.80901699437494712</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="6"/>
+        <v>0.30901699437494817</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="7"/>
+        <v>0.95105651629515364</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="7"/>
+        <v>0.5877852522924728</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="7"/>
+        <v>-0.58778525229247358</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="7"/>
+        <v>-0.95105651629515331</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f t="array" ref="A44:E44">TRANSPOSE(MMULT(B37:F41,TRANSPOSE(A32:E32)))</f>
+        <v>57.958951428993458</v>
+      </c>
+      <c r="B44" s="1">
+        <v>114.87874551770636</v>
+      </c>
+      <c r="C44" s="1">
+        <v>23.206866147101934</v>
+      </c>
+      <c r="D44" s="1">
+        <v>23.206866147101906</v>
+      </c>
+      <c r="E44" s="1">
+        <v>114.87874551770648</v>
+      </c>
+      <c r="F44" s="2">
+        <f t="array" ref="F44:J44">TRANSPOSE(MMULT(B37:F41,TRANSPOSE(F32:J32)))</f>
+        <v>-200.73430114025876</v>
+      </c>
+      <c r="G44" s="2">
+        <v>46.402295801884762</v>
+      </c>
+      <c r="H44" s="2">
+        <v>-139.33863873616917</v>
+      </c>
+      <c r="I44" s="2">
+        <v>-139.33863873616906</v>
+      </c>
+      <c r="J44" s="2">
+        <v>46.402295801884847</v>
+      </c>
+      <c r="K44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f t="array" ref="A45:E45">TRANSPOSE(MMULT(B37:F41,TRANSPOSE(A33:E33)))</f>
+        <v>-406.09090398660692</v>
+      </c>
+      <c r="B45" s="1">
+        <v>-41.016719869682873</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44.100012526963724</v>
+      </c>
+      <c r="D45" s="1">
+        <v>44.100012526963773</v>
+      </c>
+      <c r="E45" s="1">
+        <v>-41.016719869682944</v>
+      </c>
+      <c r="F45" s="2">
+        <f t="array" ref="F45:J45">TRANSPOSE(MMULT(B37:F41,TRANSPOSE(F33:J33)))</f>
+        <v>-5.9331806051585261</v>
+      </c>
+      <c r="G45" s="2">
+        <v>204.45744661548633</v>
+      </c>
+      <c r="H45" s="2">
+        <v>-105.27938064621843</v>
+      </c>
+      <c r="I45" s="2">
+        <v>-105.27938064621839</v>
+      </c>
+      <c r="J45" s="2">
+        <v>204.45744661548633</v>
+      </c>
+      <c r="K45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f t="array" ref="A46:E46">TRANSPOSE(MMULT(I37:M41,TRANSPOSE(A32:E32)))</f>
+        <v>0</v>
+      </c>
+      <c r="B46" s="1">
+        <v>128.38162195904107</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-71.601001433755883</v>
+      </c>
+      <c r="D46" s="1">
+        <v>71.601001433755869</v>
+      </c>
+      <c r="E46" s="1">
+        <v>-128.38162195904104</v>
+      </c>
+      <c r="F46" s="2">
+        <f t="array" ref="F46:J46">TRANSPOSE(MMULT(I37:M41,TRANSPOSE(F32:J32)))</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>145.91209996480765</v>
+      </c>
+      <c r="H46" s="2">
+        <v>163.51857533726997</v>
+      </c>
+      <c r="I46" s="2">
+        <v>-163.51857533727002</v>
+      </c>
+      <c r="J46" s="2">
+        <v>-145.91209996480754</v>
+      </c>
+      <c r="K46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f t="array" ref="A47:E47">TRANSPOSE(MMULT(I37:M41,TRANSPOSE(A33:E33)))</f>
+        <v>0</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-7.0082599874459675</v>
+      </c>
+      <c r="C47" s="1">
+        <v>115.25982969085037</v>
+      </c>
+      <c r="D47" s="1">
+        <v>-115.25982969085031</v>
+      </c>
+      <c r="E47" s="1">
+        <v>7.0082599874460101</v>
+      </c>
+      <c r="F47" s="2">
+        <f t="array" ref="F47:J47">TRANSPOSE(MMULT(I37:M41,TRANSPOSE(F33:J33)))</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>-86.073497355445113</v>
+      </c>
+      <c r="H47" s="2">
+        <v>17.262786404947761</v>
+      </c>
+      <c r="I47" s="2">
+        <v>-17.262786404947828</v>
+      </c>
+      <c r="J47" s="2">
+        <v>86.073497355445241</v>
+      </c>
+      <c r="K47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f>A44-A47</f>
+        <v>57.958951428993458</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ref="B52:J52" si="9">B44-B47</f>
+        <v>121.88700550515233</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="9"/>
+        <v>-92.052963543748433</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="9"/>
+        <v>138.46669583795222</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="9"/>
+        <v>107.87048553026047</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="9"/>
+        <v>-200.73430114025876</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="9"/>
+        <v>132.47579315732986</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="9"/>
+        <v>-156.60142514111692</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="9"/>
+        <v>-122.07585233122123</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="9"/>
+        <v>-39.671201553560394</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f>A45+A46</f>
+        <v>-406.09090398660692</v>
+      </c>
+      <c r="B53">
+        <f t="shared" ref="B53:J53" si="10">B45+B46</f>
+        <v>87.364902089358196</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="10"/>
+        <v>-27.500988906792159</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="10"/>
+        <v>115.70101396071965</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="10"/>
+        <v>-169.39834182872397</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="10"/>
+        <v>-5.9331806051585261</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="10"/>
+        <v>350.36954658029401</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="10"/>
+        <v>58.239194691051537</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="10"/>
+        <v>-268.79795598348841</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="10"/>
+        <v>58.545346650678795</v>
+      </c>
+      <c r="K53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:H13"/>
+      <selection activeCell="B12" sqref="B12:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3176,1381 +5192,1381 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*256-128</f>
-        <v>-82.658595982563298</v>
+        <v>112.43423914062831</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:K16" ca="1" si="0">RAND()*256-128</f>
-        <v>-24.636956967373749</v>
+        <v>36.264613100435696</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>80.643481916166309</v>
+        <v>-26.992887604621984</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>104.27903193772337</v>
+        <v>-53.556260365161762</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>-47.049411604327588</v>
+        <v>41.169382565219991</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>38.170398578129465</v>
+        <v>-74.71874581060402</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>88.302317665672433</v>
+        <v>103.96948838960458</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>87.740497796241812</v>
+        <v>-2.4259628686274937</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-70.335452002680768</v>
+        <v>126.51866953051018</v>
       </c>
       <c r="J1">
         <f t="shared" ca="1" si="0"/>
-        <v>60.778677125830853</v>
+        <v>-23.08681184056573</v>
       </c>
       <c r="K1">
         <f t="shared" ca="1" si="0"/>
-        <v>13.768702635112646</v>
+        <v>34.147611926773067</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:K30" ca="1" si="1">RAND()*256-128</f>
-        <v>99.299565445463401</v>
+        <v>-77.634187462251163</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>41.126921154925327</v>
+        <v>103.97257872427505</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>-99.344899276068048</v>
+        <v>63.035677423685854</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>75.755422227322811</v>
+        <v>-93.189519367409645</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>92.456213627177419</v>
+        <v>-66.93200001058878</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.960396142849618</v>
+        <v>27.306616642583577</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>126.11479228838721</v>
+        <v>-123.77263562624967</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.286083292816727</v>
+        <v>-17.035289397514276</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>73.430262875033009</v>
+        <v>96.674541669313214</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>99.316587895321902</v>
+        <v>-96.119881069042322</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>108.68955955719036</v>
+        <v>48.78597791852269</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>-80.629090954974401</v>
+        <v>8.48617242746991</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>42.164610035298125</v>
+        <v>-1.8577089519006051</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-48.873247089802874</v>
+        <v>106.35157609679027</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-100.23911498692627</v>
+        <v>112.62829774187367</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>113.97682140974931</v>
+        <v>-34.871922990337339</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.33908669666959668</v>
+        <v>-16.26153270205009</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>92.648310626251856</v>
+        <v>-126.3395830135313</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>19.821512196331383</v>
+        <v>47.157709111007279</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>45.405295774244479</v>
+        <v>-78.645875329442504</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>-115.19748523147553</v>
+        <v>-91.614104303794619</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>-123.35244189452354</v>
+        <v>101.69854367413183</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>40.09332403570798</v>
+        <v>48.535653613508345</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-104.80943627960832</v>
+        <v>74.58706062305555</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-115.40991224907489</v>
+        <v>63.172918171827604</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-111.21493096816596</v>
+        <v>-14.453163627699752</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>116.20731647545756</v>
+        <v>44.004383648709762</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>37.774598884317783</v>
+        <v>90.773397333103787</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.635676816221121</v>
+        <v>51.994774628724372</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.661842824942084</v>
+        <v>105.91182652616877</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>94.462474770748457</v>
+        <v>81.563852543435985</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>86.914445819072427</v>
+        <v>-4.2034784225955946</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.439669498578496</v>
+        <v>91.15649837796397</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>55.800059565293509</v>
+        <v>-125.15603489875485</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>91.29828038830118</v>
+        <v>15.422980103339825</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.4190391544895533</v>
+        <v>35.96226973031284</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.99028353779596</v>
+        <v>-96.721362955323912</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>46.074024083404254</v>
+        <v>44.422236843706401</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-73.72753594742764</v>
+        <v>105.89047534580686</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>17.501769865184599</v>
+        <v>-121.71074897860709</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>-127.14948290999396</v>
+        <v>-125.82949332993618</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>-78.281534029778385</v>
+        <v>-66.701950378793612</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>-45.624413205677541</v>
+        <v>73.484676916201124</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>-21.572554312181921</v>
+        <v>-94.287280532987495</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-71.556898227851661</v>
+        <v>-80.594165104214881</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>-113.79912837122217</v>
+        <v>116.55748962107904</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>64.680320335775548</v>
+        <v>113.95869882808481</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>14.857856567566898</v>
+        <v>105.69387971537537</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>57.146690573986945</v>
+        <v>-18.202153790623612</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>-114.62709843051084</v>
+        <v>16.456864702623193</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>118.81930468530209</v>
+        <v>-7.8306274201544852</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>-118.48211945477428</v>
+        <v>-31.450843905794983</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>-104.49353247525914</v>
+        <v>-39.744330122985815</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>-90.896342718642728</v>
+        <v>48.80656006752929</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>93.063994444881189</v>
+        <v>37.66391327944163</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>90.258078900792583</v>
+        <v>-6.0883242672662732</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-94.140880152318175</v>
+        <v>50.722108787905341</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>70.499893264874061</v>
+        <v>16.335696704655504</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0797348047202036</v>
+        <v>-69.03118019962676</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>45.31347685096469</v>
+        <v>8.7270288169260368</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>39.89438565874562</v>
+        <v>28.769042132874347</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-61.353663004161831</v>
+        <v>-116.7175008755078</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.635004609928075</v>
+        <v>-26.577459895803543</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>-80.219815685354831</v>
+        <v>40.905383844849439</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>-76.96273372861873</v>
+        <v>-122.26540864077307</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>97.39732296496075</v>
+        <v>41.028362264950005</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>19.605833216716064</v>
+        <v>-122.70792129584299</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-28.612493700827173</v>
+        <v>-72.602316329045976</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>70.96220745665039</v>
+        <v>67.120173474092212</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>124.70932036769301</v>
+        <v>89.873368938721796</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>103.52865208816354</v>
+        <v>86.915986582200674</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>105.68302611529145</v>
+        <v>37.221136536871256</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>-127.67970590964273</v>
+        <v>45.627551856728957</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>41.240388881348679</v>
+        <v>-37.269089127635908</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>-77.383887465291679</v>
+        <v>-11.394061907104401</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>-39.123230908581064</v>
+        <v>-8.5561747698401689</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>67.949664168363967</v>
+        <v>-67.638106211024194</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-109.70286539211398</v>
+        <v>-40.685845388115951</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-112.50180214340054</v>
+        <v>-77.43009771974269</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>78.499339266253003</v>
+        <v>-61.18399335866286</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.104614675162168</v>
+        <v>-25.593297333730874</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>57.29371158304653</v>
+        <v>121.06766168951995</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-62.627972921859254</v>
+        <v>-77.104171708432744</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>-51.863011706722006</v>
+        <v>4.616703743251918</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>30.672271658008384</v>
+        <v>-78.738279560160919</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>-36.45978180202232</v>
+        <v>-117.57382787040206</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>84.989134708905794</v>
+        <v>88.675260563385535</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>19.892125335799733</v>
+        <v>-53.82433206020076</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-89.064502465711058</v>
+        <v>5.2467066124831945</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-55.042816498166559</v>
+        <v>-118.18640076463987</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>58.281715675106852</v>
+        <v>-119.90475882344785</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-79.877194111457243</v>
+        <v>-88.945720972419707</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>20.147581696862431</v>
+        <v>-73.003292182514542</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>118.66081801884241</v>
+        <v>111.38781646681548</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>29.505148501685255</v>
+        <v>64.128396917821988</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>71.553073687689249</v>
+        <v>113.00126536671024</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>35.771443886865342</v>
+        <v>-100.20799604113913</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>-38.656452098195871</v>
+        <v>122.13209307908386</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>-27.455997284604422</v>
+        <v>41.058480915161198</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-95.297401033456566</v>
+        <v>-15.104580218574597</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>46.280815158059738</v>
+        <v>75.14395890295296</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>87.233456189996332</v>
+        <v>28.687890404225271</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>97.282693595791358</v>
+        <v>17.230641983316275</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>119.12564257117961</v>
+        <v>-74.08168440991119</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>84.736741485826741</v>
+        <v>24.471941396795245</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>63.300332743768081</v>
+        <v>-25.080708562364549</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>19.485034179558056</v>
+        <v>49.22582121659616</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4961917463492114</v>
+        <v>80.702293695351955</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>30.563065032243401</v>
+        <v>79.747788280381343</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>-93.284523648112923</v>
+        <v>-101.2638103844134</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>35.044665158944525</v>
+        <v>97.25661938438077</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>22.534517891685852</v>
+        <v>-121.54407996299696</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>43.888509445342976</v>
+        <v>-11.228672370545922</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>66.756105610260192</v>
+        <v>-11.049343977263106</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>34.597723955637207</v>
+        <v>19.613162153553191</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>-85.172299909076486</v>
+        <v>11.959678166328331</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>43.287760802482438</v>
+        <v>48.453284777878849</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>-54.6100940132647</v>
+        <v>99.991325244326958</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>119.21947166876109</v>
+        <v>120.02658498031673</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>126.98917637311135</v>
+        <v>-46.027388826547707</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>90.047227501907344</v>
+        <v>121.31950700447894</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-76.56912523172241</v>
+        <v>-124.8504335533828</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>44.929597990724517</v>
+        <v>-16.659064496845247</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-27.822023549827946</v>
+        <v>13.902024626088632</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-49.458442488693208</v>
+        <v>78.960371309223234</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>116.75016200231909</v>
+        <v>-67.002441974362995</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>-63.964052076420842</v>
+        <v>-122.68856085031027</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.6569054419026656</v>
+        <v>-40.910137527558106</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>-124.41711582577261</v>
+        <v>-92.617931068634334</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>82.312153442606302</v>
+        <v>-81.92844950712265</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>-65.264104858096431</v>
+        <v>-54.346159841540924</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>98.99790038692521</v>
+        <v>-113.02950042930598</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>41.288054519790222</v>
+        <v>44.424528832848239</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-42.806317795263283</v>
+        <v>-23.449269615598439</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>101.76863525276522</v>
+        <v>-66.100940695297112</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>54.570142156707249</v>
+        <v>59.539716456685852</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>27.947742643240701</v>
+        <v>33.772364464956581</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>127.79267491720705</v>
+        <v>-26.470924564784411</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-15.890333980755855</v>
+        <v>68.351973032635442</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>127.65371068711477</v>
+        <v>-15.056462835764876</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-85.009290872686449</v>
+        <v>-99.495024943080409</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>-116.81806939870927</v>
+        <v>38.741015932030194</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.727272255969325</v>
+        <v>-24.767813930773798</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>61.44736048942562</v>
+        <v>94.639936778063003</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-78.974153469641664</v>
+        <v>-82.389232427955136</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-121.97716323140546</v>
+        <v>-26.892731150493944</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>-84.775946216434534</v>
+        <v>-80.256226452150258</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>29.197965249570842</v>
+        <v>-127.85990369267373</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-120.34345566048901</v>
+        <v>27.718981896881303</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>56.613020726739194</v>
+        <v>37.757881510958725</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>18.805997654321288</v>
+        <v>-53.605595106109689</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-107.8636530165291</v>
+        <v>87.719945877223665</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>117.08445921947998</v>
+        <v>42.203043202553516</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>57.745917357106862</v>
+        <v>33.22391814378912</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>18.112268217666923</v>
+        <v>40.71463670516988</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-49.797168369911759</v>
+        <v>82.848896469637765</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-35.766883645395808</v>
+        <v>78.350837696788659</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>36.795514398132468</v>
+        <v>43.444986549022076</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-33.607118028072904</v>
+        <v>-86.348080339946904</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>-107.14035786460036</v>
+        <v>46.270777758437077</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>61.120429996709419</v>
+        <v>66.141682626097065</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>76.234864559599089</v>
+        <v>-42.842080703804754</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>-118.3069000038349</v>
+        <v>68.082494749455577</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>-49.971918500764133</v>
+        <v>32.032365884784497</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>-40.187149092563828</v>
+        <v>-113.12059619733409</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>37.667872698970598</v>
+        <v>75.259841704998479</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>55.837216604472133</v>
+        <v>17.406729096996315</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>-126.60240882274201</v>
+        <v>51.881327982998528</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-67.084558998970778</v>
+        <v>81.468768372611493</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-107.07689572897451</v>
+        <v>99.521703163519277</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>108.10209836728777</v>
+        <v>-86.677345843452883</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-109.8849219489594</v>
+        <v>94.631887091198706</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>52.343891679180359</v>
+        <v>119.04136545794441</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>121.34786394521333</v>
+        <v>59.837308899715481</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>23.137916604270913</v>
+        <v>10.333839963847026</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
-        <v>-86.725494012375378</v>
+        <v>25.853221038278605</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>13.232731065578946</v>
+        <v>8.7601646918820961</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-124.0078995050807</v>
+        <v>73.428312091372078</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-127.84360073209874</v>
+        <v>99.849784156039391</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>41.75296928457638</v>
+        <v>-88.706007959183069</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2189041566811909</v>
+        <v>55.013723174427497</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-109.40993310098906</v>
+        <v>-19.030489479362132</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-76.118511304586292</v>
+        <v>-45.12706791931501</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>121.44734689847053</v>
+        <v>86.674077582672879</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>-119.70110731753144</v>
+        <v>38.054865832956551</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="1"/>
-        <v>16.578942475554982</v>
+        <v>48.111701678084216</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="1"/>
-        <v>77.096705355596725</v>
+        <v>24.094469978688153</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>-101.97896584864171</v>
+        <v>-124.08419022464739</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.6411022001688877</v>
+        <v>-113.29146484894972</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>119.33328927987554</v>
+        <v>-69.937192448157958</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-62.418807642947002</v>
+        <v>96.431897181148202</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>54.290220469603582</v>
+        <v>96.109306846287126</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>-114.93555509968127</v>
+        <v>-49.583966527154615</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>-118.61529084484985</v>
+        <v>-51.077048165016862</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>114.25656809148958</v>
+        <v>-52.252243908417768</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>-31.341974579445917</v>
+        <v>46.166091822078187</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="1"/>
-        <v>-43.575416045630561</v>
+        <v>63.737165882274923</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="1"/>
-        <v>-22.908008255068182</v>
+        <v>117.76897514562222</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>75.190135392809026</v>
+        <v>-73.752192941886619</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-124.76497762231716</v>
+        <v>88.483792165097384</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-45.401007836400879</v>
+        <v>115.11193493873375</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>94.172443190938964</v>
+        <v>-59.173294585493068</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-48.695358927830455</v>
+        <v>-72.844102528534165</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-35.82522792318079</v>
+        <v>52.633169499889249</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>17.657940947519762</v>
+        <v>32.662750066249686</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>70.367214008081561</v>
+        <v>84.006798353080171</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>-28.407170871902281</v>
+        <v>34.130243011018109</v>
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="1"/>
-        <v>85.546746296230566</v>
+        <v>77.036673763753981</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.438072471257129</v>
+        <v>112.03809046324182</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>58.296588826786916</v>
+        <v>98.358203784192483</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>60.564356483681195</v>
+        <v>-122.51322596488012</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.4417722993547102</v>
+        <v>108.96180753981639</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>-89.043875846039725</v>
+        <v>-90.972065555127955</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>12.071351636258072</v>
+        <v>11.066025805724735</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>-26.710006856537149</v>
+        <v>-57.178021365609993</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>-42.355083860108152</v>
+        <v>35.796205348755905</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>29.995675669991385</v>
+        <v>126.24747334300562</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>127.24221756680979</v>
+        <v>11.776700517266676</v>
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="1"/>
-        <v>15.285358900089335</v>
+        <v>-56.479237412388585</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="1"/>
-        <v>92.331673686108644</v>
+        <v>2.2583014807865993</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>106.98984437073824</v>
+        <v>-100.55882658359926</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>-75.650482903079961</v>
+        <v>7.0936323424569991</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>64.900922227830165</v>
+        <v>-42.624407645608926</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>41.050831174982108</v>
+        <v>4.1572447469296208</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>33.818410035313889</v>
+        <v>27.044765442658672</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>62.88697576530069</v>
+        <v>-35.586099054144682</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>-93.27904574994119</v>
+        <v>36.982337126489369</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>-116.57285009333137</v>
+        <v>-5.2622095067933401</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>103.81780136042633</v>
+        <v>-95.526051058829836</v>
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>71.094072516360484</v>
+        <v>-23.926202366106992</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
-        <v>18.973813550488245</v>
+        <v>33.631507295393163</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>116.2658361122414</v>
+        <v>-99.801829676493867</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>61.394875858001512</v>
+        <v>34.230876723507464</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>59.363370356378454</v>
+        <v>-69.415074986453021</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>61.583677522731506</v>
+        <v>-7.8105113184890627</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>72.44398738718138</v>
+        <v>39.793585135842079</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>51.552361537576672</v>
+        <v>123.86917965335618</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>100.46574361603786</v>
+        <v>89.070434788513097</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>85.106208371018965</v>
+        <v>-80.872565533324803</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>-38.518745247937744</v>
+        <v>48.612607352012617</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>-76.742245473051213</v>
+        <v>83.563216049886307</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.848257294608203</v>
+        <v>19.630315150780604</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>38.129240198545091</v>
+        <v>-57.49481087838214</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>-119.87451248751847</v>
+        <v>-108.46161757731019</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>-105.44469842525746</v>
+        <v>70.941478813858566</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>-12.134549323232648</v>
+        <v>-122.94804998413304</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>-75.415651799687026</v>
+        <v>-47.871619917181647</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>56.751368301077321</v>
+        <v>53.694742290775054</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-91.249556269196944</v>
+        <v>114.84737003534167</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.0642636553282045</v>
+        <v>-115.16956993447127</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>22.627167989317456</v>
+        <v>-84.934631616936514</v>
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>84.163828711075411</v>
+        <v>89.237202255606974</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
-        <v>72.56790020729278</v>
+        <v>-84.792145047706697</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.605521500185063</v>
+        <v>69.394116831740234</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>-115.74626336913326</v>
+        <v>-64.950529348121876</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>-72.142984031451022</v>
+        <v>63.955539149642362</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>38.380855957539666</v>
+        <v>-82.636560061700067</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>43.623524095832238</v>
+        <v>78.513044776911613</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-88.935594957450462</v>
+        <v>40.568786080647868</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>99.293132714088983</v>
+        <v>97.355630933779111</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>-60.69759858673504</v>
+        <v>-2.279425106125359</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>-110.63790271007994</v>
+        <v>-40.838366276356822</v>
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>55.330425978526819</v>
+        <v>-124.15289422494243</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
-        <v>66.594554247123597</v>
+        <v>-18.887517440509924</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>83.877835106712467</v>
+        <v>74.652201135177393</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>59.508055869629345</v>
+        <v>44.441313116189519</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>-77.942748622278771</v>
+        <v>-50.067199667998096</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>62.815491139049499</v>
+        <v>68.257280612545259</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>30.405101557493225</v>
+        <v>-37.063300181922642</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>25.516960777510661</v>
+        <v>106.48782944215893</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>78.443928416995533</v>
+        <v>90.549462829402358</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>25.497924906483689</v>
+        <v>-77.335400307365092</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
-        <v>-107.34744919448801</v>
+        <v>25.270617679850318</v>
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>72.111923464870728</v>
+        <v>3.3087181034534865</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.074929193786119</v>
+        <v>-35.296682175944284</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>63.1632926963008</v>
+        <v>-90.025330678979657</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8206069898160138</v>
+        <v>72.324506876783062</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>92.154789331342641</v>
+        <v>-22.172904138655667</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0839163280500657</v>
+        <v>50.335668001675231</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>53.948299892419385</v>
+        <v>46.211654302688771</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>62.31203959473703</v>
+        <v>-123.68968140157816</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>112.9132190043031</v>
+        <v>-91.416532234749752</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>-81.389288247764341</v>
+        <v>74.715252734498364</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
-        <v>-114.1463665840391</v>
+        <v>-72.625259621869674</v>
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>81.563620491451644</v>
+        <v>27.0615394517026</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="1"/>
-        <v>-35.311760626025972</v>
+        <v>-69.503229279441399</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>26.860132990254272</v>
+        <v>121.06777892119101</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3909607513137132</v>
+        <v>45.008149115111422</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>44.332817314682643</v>
+        <v>48.799661034430301</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>33.929303237832983</v>
+        <v>17.918112046554654</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.03804030988988</v>
+        <v>-102.77493832026212</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>43.441504941425706</v>
+        <v>55.661376781237209</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>57.134668847613909</v>
+        <v>43.413402308200858</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>-100.43085215554473</v>
+        <v>-63.297607096374719</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
-        <v>-24.827495028169238</v>
+        <v>-8.4491603510149105</v>
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>51.074376421334961</v>
+        <v>-48.303946960130332</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="1"/>
-        <v>-90.315642815846729</v>
+        <v>108.38019589699852</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>-35.303072144800012</v>
+        <v>54.158458530606282</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>-28.729751011199795</v>
+        <v>87.862866720585515</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66672704048301057</v>
+        <v>70.715592166790344</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.6969698361345422</v>
+        <v>111.96287443478016</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>41.614396329410056</v>
+        <v>-15.938361314742508</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>-100.71892371841415</v>
+        <v>-47.564135568219768</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>53.856999461419065</v>
+        <v>-91.207895448875917</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>76.218507451292936</v>
+        <v>36.579108687139211</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.4376527943476844</v>
+        <v>-33.010708962610153</v>
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="1"/>
-        <v>42.441883323436798</v>
+        <v>33.115250167366469</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8664362031431665</v>
+        <v>9.3905047806481434</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>60.502237893490673</v>
+        <v>108.09699808804501</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.631946920304614</v>
+        <v>63.808729347275914</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>-78.450357641969163</v>
+        <v>26.922306341410973</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>30.913689582913008</v>
+        <v>-119.58573847043942</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>97.998286403582199</v>
+        <v>-34.938370152991951</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>-82.434833721002917</v>
+        <v>110.84850633877522</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>45.169645689738815</v>
+        <v>114.2537525083323</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>-58.310366402398699</v>
+        <v>-19.299760456896223</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="1"/>
-        <v>-35.401035326062271</v>
+        <v>27.599181752342105</v>
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="1"/>
-        <v>-66.703768346529529</v>
+        <v>-103.40757536672143</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="1"/>
-        <v>25.337527484306662</v>
+        <v>39.051612283530346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>